<commit_message>
Base function for creating new xlsx file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Programming languages and methods\Draughts-Tournament-Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAD1976-57A9-43D6-B23D-23FF64554C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6D48A5C-7D55-4A67-AA6C-C0108C72841E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Основная таблица" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
+    <sheet name="Турнирные данные" sheetId="2" r:id="rId2"/>
+    <sheet name="Туры" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="94">
   <si>
     <t>Иванов Иван</t>
   </si>
@@ -230,6 +232,84 @@
   </si>
   <si>
     <t>1b9</t>
+  </si>
+  <si>
+    <t>Турнир посвященный Новому году</t>
+  </si>
+  <si>
+    <t>Малахов Сергей Сергеевич</t>
+  </si>
+  <si>
+    <t>Максимов Алексей Павлович</t>
+  </si>
+  <si>
+    <t>Швейцарская</t>
+  </si>
+  <si>
+    <t>Личная встреча</t>
+  </si>
+  <si>
+    <t>Коэффициент Шмульяна</t>
+  </si>
+  <si>
+    <t>Количество побед</t>
+  </si>
+  <si>
+    <t>Коэффициент Бухгольца</t>
+  </si>
+  <si>
+    <t>Название турнира:</t>
+  </si>
+  <si>
+    <t>ФИО судьи:</t>
+  </si>
+  <si>
+    <t>ФИО помощника судьи:</t>
+  </si>
+  <si>
+    <t>Система проведения соревнований:</t>
+  </si>
+  <si>
+    <t>Количество туров:</t>
+  </si>
+  <si>
+    <t>Номер текущего тура:</t>
+  </si>
+  <si>
+    <t>Дата начала соревнований:</t>
+  </si>
+  <si>
+    <t>Дата окончания соревнований:</t>
+  </si>
+  <si>
+    <t>Приоритет 1 при равенстве очков:</t>
+  </si>
+  <si>
+    <t>Приоритет 2 при равенстве очков:</t>
+  </si>
+  <si>
+    <t>Приоритет 3 при равенстве очков:</t>
+  </si>
+  <si>
+    <t>Приоритет 4 при равенстве очков:</t>
+  </si>
+  <si>
+    <t>Игрок белым цветом</t>
+  </si>
+  <si>
+    <t>Игрок черным цветом</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>2 -- 0</t>
+  </si>
+  <si>
+    <t>1 -- 1</t>
+  </si>
+  <si>
+    <t>0 -- 2</t>
   </si>
 </sst>
 </file>
@@ -271,9 +351,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -557,7 +639,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,12 +1364,318 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAEC4A9-A85E-445C-9811-1E32520FF4B7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5A2568-A2EB-46DC-BFBE-3BF2378CFD1D}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>